<commit_message>
Bump five 68552 variants to 178 pcs to clear 50 GP threshold
- 68552-20/40/80/160/320 now at 178 pcs, 54 GP each
- Viable lines: 39 -> 44, Total GP: 3,491
</commit_message>
<xml_diff>
--- a/Trading Analysis/LAM review/Lam-Astute_NewParts - Completed.xlsx
+++ b/Trading Analysis/LAM review/Lam-Astute_NewParts - Completed.xlsx
@@ -2656,7 +2656,7 @@
         <v>445</v>
       </c>
       <c r="G24" s="3" t="n">
-        <v>125</v>
+        <v>178</v>
       </c>
       <c r="H24" s="2" t="inlineStr"/>
       <c r="I24" s="4" t="n">
@@ -2683,12 +2683,12 @@
       <c r="R24" s="5" t="n">
         <v>634.3919999999999</v>
       </c>
-      <c r="S24" s="5" t="n">
-        <v>178.2</v>
-      </c>
-      <c r="T24" s="7" t="inlineStr">
-        <is>
-          <t>NO</t>
+      <c r="S24" s="8" t="n">
+        <v>253.7568</v>
+      </c>
+      <c r="T24" s="9" t="inlineStr">
+        <is>
+          <t>YES</t>
         </is>
       </c>
       <c r="U24" s="2" t="inlineStr">
@@ -2743,7 +2743,7 @@
         <v>445</v>
       </c>
       <c r="G25" s="3" t="n">
-        <v>125</v>
+        <v>178</v>
       </c>
       <c r="H25" s="2" t="inlineStr"/>
       <c r="I25" s="4" t="n">
@@ -2770,12 +2770,12 @@
       <c r="R25" s="5" t="n">
         <v>634.3919999999999</v>
       </c>
-      <c r="S25" s="5" t="n">
-        <v>178.2</v>
-      </c>
-      <c r="T25" s="7" t="inlineStr">
-        <is>
-          <t>NO</t>
+      <c r="S25" s="8" t="n">
+        <v>253.7568</v>
+      </c>
+      <c r="T25" s="9" t="inlineStr">
+        <is>
+          <t>YES</t>
         </is>
       </c>
       <c r="U25" s="2" t="inlineStr">
@@ -2830,7 +2830,7 @@
         <v>445</v>
       </c>
       <c r="G26" s="3" t="n">
-        <v>125</v>
+        <v>178</v>
       </c>
       <c r="H26" s="2" t="inlineStr"/>
       <c r="I26" s="4" t="n">
@@ -2857,12 +2857,12 @@
       <c r="R26" s="5" t="n">
         <v>634.3919999999999</v>
       </c>
-      <c r="S26" s="5" t="n">
-        <v>178.2</v>
-      </c>
-      <c r="T26" s="7" t="inlineStr">
-        <is>
-          <t>NO</t>
+      <c r="S26" s="8" t="n">
+        <v>253.7568</v>
+      </c>
+      <c r="T26" s="9" t="inlineStr">
+        <is>
+          <t>YES</t>
         </is>
       </c>
       <c r="U26" s="2" t="inlineStr">
@@ -2917,7 +2917,7 @@
         <v>445</v>
       </c>
       <c r="G27" s="3" t="n">
-        <v>125</v>
+        <v>178</v>
       </c>
       <c r="H27" s="2" t="inlineStr"/>
       <c r="I27" s="4" t="n">
@@ -2944,12 +2944,12 @@
       <c r="R27" s="5" t="n">
         <v>634.3919999999999</v>
       </c>
-      <c r="S27" s="5" t="n">
-        <v>178.2</v>
-      </c>
-      <c r="T27" s="7" t="inlineStr">
-        <is>
-          <t>NO</t>
+      <c r="S27" s="8" t="n">
+        <v>253.7568</v>
+      </c>
+      <c r="T27" s="9" t="inlineStr">
+        <is>
+          <t>YES</t>
         </is>
       </c>
       <c r="U27" s="2" t="inlineStr">
@@ -3004,7 +3004,7 @@
         <v>445</v>
       </c>
       <c r="G28" s="3" t="n">
-        <v>125</v>
+        <v>178</v>
       </c>
       <c r="H28" s="2" t="inlineStr"/>
       <c r="I28" s="4" t="n">
@@ -3031,12 +3031,12 @@
       <c r="R28" s="5" t="n">
         <v>634.3919999999999</v>
       </c>
-      <c r="S28" s="5" t="n">
-        <v>178.2</v>
-      </c>
-      <c r="T28" s="7" t="inlineStr">
-        <is>
-          <t>NO</t>
+      <c r="S28" s="8" t="n">
+        <v>253.7568</v>
+      </c>
+      <c r="T28" s="9" t="inlineStr">
+        <is>
+          <t>YES</t>
         </is>
       </c>
       <c r="U28" s="2" t="inlineStr">

</xml_diff>